<commit_message>
Criação do Relatório de Orçamento
Implantação de relatório do orçado, Clayton
</commit_message>
<xml_diff>
--- a/Plano de Trabalho.xlsx
+++ b/Plano de Trabalho.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clayton\OneDrive - URBANVIX URBANIZADORA E INCORPORADORA LTDA\Documentos\GitHub\fullhouse-Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D423E1-423F-4281-9962-6C1D51343F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084412A-EA20-492B-8CFD-83A2F4096EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{A7B32508-10FC-4821-A85C-AB803D040999}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Trabalho" sheetId="1" r:id="rId1"/>
+    <sheet name="Observações" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="110">
   <si>
     <t>Dashboard</t>
   </si>
@@ -345,14 +346,23 @@
     <t>Menu</t>
   </si>
   <si>
-    <t>Criação Grá</t>
+    <t>Exportar Lançamentos já feitos para excel</t>
+  </si>
+  <si>
+    <t>Andamento</t>
+  </si>
+  <si>
+    <t>Criação Gráfico</t>
+  </si>
+  <si>
+    <t>Jaque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,6 +406,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -417,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -427,15 +451,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,11 +778,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F7E6C5-D897-41B1-9711-E9EB77ED7C2E}">
-  <dimension ref="B1:L101"/>
+  <dimension ref="B1:L103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -769,39 +797,39 @@
     <col min="8" max="8" width="2.5703125" style="1" customWidth="1"/>
     <col min="9" max="10" width="12.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="6"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="9"/>
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -821,6 +849,9 @@
       <c r="G5" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="K5" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
@@ -832,6 +863,9 @@
       <c r="G6" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="K6" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
@@ -869,16 +903,16 @@
       <c r="G13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>45657</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>45716</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="8" t="s">
         <v>91</v>
       </c>
     </row>
@@ -892,10 +926,10 @@
       <c r="G14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>45657</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <v>45716</v>
       </c>
       <c r="K14" s="4" t="s">
@@ -912,10 +946,10 @@
       <c r="G15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>45657</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>45716</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -979,7 +1013,13 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
@@ -994,6 +1034,9 @@
       <c r="E24" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G24" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
@@ -1002,6 +1045,9 @@
       <c r="E25" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G25" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
@@ -1010,6 +1056,9 @@
       <c r="E26" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G26" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
@@ -1018,6 +1067,9 @@
       <c r="E27" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G27" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
@@ -1026,6 +1078,9 @@
       <c r="E28" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G28" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
@@ -1034,6 +1089,9 @@
       <c r="E29" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G29" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
@@ -1042,6 +1100,9 @@
       <c r="E30" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="G30" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
@@ -1055,6 +1116,9 @@
       <c r="E33" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G33" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C34" s="1" t="s">
@@ -1063,6 +1127,9 @@
       <c r="E34" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G34" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C35" s="1" t="s">
@@ -1071,10 +1138,13 @@
       <c r="E35" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G35" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>93</v>
@@ -1082,26 +1152,29 @@
       <c r="G36" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="L36" s="9" t="s">
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L37" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B38" s="2" t="s">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C40" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>27</v>
@@ -1109,7 +1182,7 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>27</v>
@@ -1117,7 +1190,7 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>27</v>
@@ -1125,7 +1198,7 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>27</v>
@@ -1133,7 +1206,7 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>27</v>
@@ -1141,7 +1214,7 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>27</v>
@@ -1149,7 +1222,7 @@
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>27</v>
@@ -1157,7 +1230,7 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C47" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>27</v>
@@ -1165,241 +1238,254 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C50" s="1" t="s">
+      <c r="E50" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C52" s="1" t="s">
+      <c r="E52" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C53" s="1" t="s">
+      <c r="E53" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C54" s="1" t="s">
+      <c r="E54" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C55" s="1" t="s">
+      <c r="E55" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C56" s="1" t="s">
+      <c r="E56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="7">
+        <v>45740</v>
+      </c>
+      <c r="J56" s="7">
+        <v>45741</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C57" s="1" t="s">
+      <c r="E57" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C58" s="1" t="s">
+      <c r="E58" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C59" s="1" t="s">
+      <c r="E59" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C61" s="1" t="s">
+      <c r="E61" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B63" s="2" t="s">
+      <c r="E62" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B65" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C64" s="1" t="s">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C65" s="1" t="s">
+      <c r="E66" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C66" s="1" t="s">
+      <c r="E67" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C67" s="1" t="s">
+      <c r="E68" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C68" s="1" t="s">
+      <c r="E69" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C69" s="1" t="s">
+      <c r="E70" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C70" s="1" t="s">
+      <c r="E71" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C71" s="1" t="s">
+      <c r="E72" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C72" s="1" t="s">
+      <c r="E73" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C73" s="1" t="s">
+      <c r="E74" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C74" s="1" t="s">
+      <c r="E75" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C75" s="1" t="s">
+      <c r="E76" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="2" t="s">
+      <c r="E77" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B79" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C78" s="1" t="s">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C79" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C80" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>27</v>
@@ -1407,7 +1493,7 @@
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C81" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>27</v>
@@ -1415,7 +1501,7 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C82" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>27</v>
@@ -1423,7 +1509,7 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C83" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>27</v>
@@ -1431,7 +1517,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C84" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>27</v>
@@ -1439,7 +1525,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C85" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>27</v>
@@ -1447,7 +1533,7 @@
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>27</v>
@@ -1455,7 +1541,7 @@
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C87" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>27</v>
@@ -1463,7 +1549,7 @@
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C88" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>27</v>
@@ -1471,36 +1557,36 @@
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C90" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C91" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E89" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B91" s="2" t="s">
+      <c r="E91" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B93" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C92" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C93" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C94" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>27</v>
@@ -1508,7 +1594,7 @@
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C95" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>27</v>
@@ -1516,47 +1602,63 @@
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C96" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C97" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C98" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E96" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B98" s="2" t="s">
+      <c r="E98" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B100" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C99" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G99" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C100" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C101" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>100</v>
       </c>
       <c r="G101" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C102" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C103" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G103" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1567,4 +1669,24 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DB7A1B-1B8E-4D9D-ADE6-7393443870BE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clayton - ajustes no Simulador de Negócios
Ajuste no tamanho do campo do status, não permitir alteração da data depois de incluído, inclusão de icones e consulta da área no simulador
</commit_message>
<xml_diff>
--- a/Plano de Trabalho.xlsx
+++ b/Plano de Trabalho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clayton\OneDrive - URBANVIX URBANIZADORA E INCORPORADORA LTDA\Documentos\GitHub\fullhouse-Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084412A-EA20-492B-8CFD-83A2F4096EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E2E22-BFD4-4ECC-B13C-B4212AE19CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{A7B32508-10FC-4821-A85C-AB803D040999}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="114">
   <si>
     <t>Dashboard</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>Jaque</t>
+  </si>
+  <si>
+    <t>Anexos do Estudo de áreas</t>
+  </si>
+  <si>
+    <t>Anexar vários documentos para o estudo, index por autonumeração no banco, criar tela para checar documetnação anexada</t>
+  </si>
+  <si>
+    <t>Incluir precificação de custo SINAP/SICRO/DER/ETC</t>
+  </si>
+  <si>
+    <t>Criar APIs para baixa dos arquivos e montagem do custo programado com os código dos serviços</t>
   </si>
 </sst>
 </file>
@@ -457,13 +469,13 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,11 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F7E6C5-D897-41B1-9711-E9EB77ED7C2E}">
-  <dimension ref="B1:L103"/>
+  <dimension ref="B1:L105"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -802,16 +814,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="9"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="11"/>
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
@@ -849,7 +861,7 @@
       <c r="G5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -863,7 +875,7 @@
       <c r="G6" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="10" t="s">
         <v>107</v>
       </c>
     </row>
@@ -967,7 +979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
@@ -978,7 +990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>108</v>
       </c>
@@ -1022,36 +1034,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>27</v>
@@ -1060,9 +1078,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>27</v>
@@ -1071,9 +1089,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>27</v>
@@ -1082,9 +1100,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>27</v>
@@ -1093,47 +1111,47 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="2" t="s">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>27</v>
@@ -1144,53 +1162,59 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>93</v>
+        <v>27</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="C39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="L37" s="8" t="s">
+      <c r="L39" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B39" s="2" t="s">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C42" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>27</v>
@@ -1198,7 +1222,7 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>27</v>
@@ -1206,7 +1230,7 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>27</v>
@@ -1214,7 +1238,7 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>27</v>
@@ -1222,7 +1246,7 @@
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C46" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>27</v>
@@ -1230,7 +1254,7 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>27</v>
@@ -1238,7 +1262,7 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>27</v>
@@ -1246,7 +1270,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>27</v>
@@ -1254,7 +1278,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C50" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>27</v>
@@ -1262,7 +1286,7 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C51" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>27</v>
@@ -1270,7 +1294,7 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>27</v>
@@ -1278,7 +1302,7 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>27</v>
@@ -1286,7 +1310,7 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C54" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>27</v>
@@ -1294,7 +1318,7 @@
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>27</v>
@@ -1302,27 +1326,15 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C56" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" s="7">
-        <v>45740</v>
-      </c>
-      <c r="J56" s="7">
-        <v>45741</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>27</v>
@@ -1330,15 +1342,27 @@
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I58" s="7">
+        <v>45740</v>
+      </c>
+      <c r="J58" s="7">
+        <v>45741</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C59" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>27</v>
@@ -1346,18 +1370,15 @@
     </row>
     <row r="60" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C60" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C61" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>27</v>
@@ -1365,47 +1386,50 @@
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C63" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C64" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B65" s="2" t="s">
+      <c r="E64" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B67" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C67" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>27</v>
@@ -1413,7 +1437,7 @@
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>27</v>
@@ -1421,7 +1445,7 @@
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>27</v>
@@ -1429,7 +1453,7 @@
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>27</v>
@@ -1437,7 +1461,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>27</v>
@@ -1445,7 +1469,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>27</v>
@@ -1453,18 +1477,15 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>27</v>
@@ -1472,36 +1493,39 @@
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B79" s="2" t="s">
+      <c r="E79" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B81" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C80" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C82" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>27</v>
@@ -1509,7 +1533,7 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C83" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>27</v>
@@ -1517,7 +1541,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C84" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>27</v>
@@ -1525,7 +1549,7 @@
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C85" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>27</v>
@@ -1533,7 +1557,7 @@
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>27</v>
@@ -1541,7 +1565,7 @@
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C87" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>27</v>
@@ -1549,7 +1573,7 @@
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C88" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>27</v>
@@ -1557,7 +1581,7 @@
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C89" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>27</v>
@@ -1565,7 +1589,7 @@
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C90" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>27</v>
@@ -1573,36 +1597,36 @@
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C91" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C92" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C93" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E91" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B93" s="2" t="s">
+      <c r="E93" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B95" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C94" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="C95" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C96" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>27</v>
@@ -1610,7 +1634,7 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C97" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>27</v>
@@ -1618,47 +1642,63 @@
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C98" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C99" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C100" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B100" s="2" t="s">
+      <c r="E100" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B102" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C101" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C102" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G102" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C103" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>100</v>
       </c>
       <c r="G103" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C104" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C105" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G105" s="4" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Criação do Atualizador de versão
</commit_message>
<xml_diff>
--- a/Plano de Trabalho.xlsx
+++ b/Plano de Trabalho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clayton\OneDrive - URBANVIX URBANIZADORA E INCORPORADORA LTDA\Documentos\GitHub\fullhouse-Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1E2E22-BFD4-4ECC-B13C-B4212AE19CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5B7870-8FFA-463F-93A5-8449B3F9BEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{A7B32508-10FC-4821-A85C-AB803D040999}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t>Dashboard</t>
   </si>
@@ -361,13 +361,22 @@
     <t>Anexos do Estudo de áreas</t>
   </si>
   <si>
-    <t>Anexar vários documentos para o estudo, index por autonumeração no banco, criar tela para checar documetnação anexada</t>
-  </si>
-  <si>
     <t>Incluir precificação de custo SINAP/SICRO/DER/ETC</t>
   </si>
   <si>
     <t>Criar APIs para baixa dos arquivos e montagem do custo programado com os código dos serviços</t>
+  </si>
+  <si>
+    <t>* alterar o valor do Terreno para negativo</t>
+  </si>
+  <si>
+    <t>Anexar vários documentos para o estudo, index por autonumeração no banco, criar tela para checar documetnação anexada. Criar um tela para ver todos os documentos anexados, o indice será a empresa, uf. Município, Nome do Cenário todos os documentos ficarão vinculados aos cenários de forma única</t>
+  </si>
+  <si>
+    <t>Alterar a chave de pesquisa, retirando o tipo e deixando somente pela empresa, uf, cidade</t>
+  </si>
+  <si>
+    <t>* Criar status lixeira</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -473,6 +482,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,7 +807,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -814,16 +827,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="13"/>
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
@@ -947,25 +960,34 @@
       <c r="K14" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="L14" s="8" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="D15" s="8"/>
+      <c r="E15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="12">
         <v>45657</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="12">
         <v>45716</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="11" t="s">
         <v>24</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
@@ -1022,6 +1044,9 @@
       <c r="G20" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="L20" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
@@ -1045,12 +1070,12 @@
         <v>20</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>100</v>
@@ -1059,7 +1084,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Cronograma - Ajustes Finos
</commit_message>
<xml_diff>
--- a/Plano de Trabalho.xlsx
+++ b/Plano de Trabalho.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clayton\OneDrive - URBANVIX URBANIZADORA E INCORPORADORA LTDA\Documentos\GitHub\fullhouse-Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5B7870-8FFA-463F-93A5-8449B3F9BEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFA3B68-468B-4E9A-9ED3-1EFB0AF7DEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{A7B32508-10FC-4821-A85C-AB803D040999}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7B32508-10FC-4821-A85C-AB803D040999}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Trabalho" sheetId="1" r:id="rId1"/>
     <sheet name="Observações" sheetId="2" r:id="rId2"/>
+    <sheet name="Modelo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="139">
   <si>
     <t>Dashboard</t>
   </si>
@@ -377,13 +378,79 @@
   </si>
   <si>
     <t>* Criar status lixeira</t>
+  </si>
+  <si>
+    <t>Alterar as mensagens para usuários</t>
+  </si>
+  <si>
+    <t>Ajustes finos</t>
+  </si>
+  <si>
+    <t>Clayton fazer modelo de tela e encaminhar para jaque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Vcto </t>
+  </si>
+  <si>
+    <t>Inicial</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Fornecedor/Cliente</t>
+  </si>
+  <si>
+    <t>A receber ou a pagar</t>
+  </si>
+  <si>
+    <t>Nr do Documento</t>
+  </si>
+  <si>
+    <t>Valor do titulo</t>
+  </si>
+  <si>
+    <t>Vcnto</t>
+  </si>
+  <si>
+    <t>Informações Liquidação</t>
+  </si>
+  <si>
+    <t>Boleto se é pix se deposito</t>
+  </si>
+  <si>
+    <t>Todos, em aberto, liquidados</t>
+  </si>
+  <si>
+    <t>Dta Liquidação</t>
+  </si>
+  <si>
+    <t>Origem</t>
+  </si>
+  <si>
+    <t>A pagar</t>
+  </si>
+  <si>
+    <t>ou</t>
+  </si>
+  <si>
+    <t>A receber</t>
+  </si>
+  <si>
+    <t>Origem:</t>
+  </si>
+  <si>
+    <t>Situação:</t>
+  </si>
+  <si>
+    <t>Modelo *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,13 +508,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF76E3FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -462,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,6 +576,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,7 +900,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1102,6 +1195,9 @@
       <c r="G26" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L26" s="8" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
@@ -1113,6 +1209,9 @@
       <c r="G27" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L27" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
@@ -1124,6 +1223,9 @@
       <c r="G28" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L28" s="8" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
@@ -1135,6 +1237,9 @@
       <c r="G29" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L29" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
@@ -1146,6 +1251,9 @@
       <c r="G30" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L30" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
@@ -1157,6 +1265,9 @@
       <c r="G31" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="L31" s="8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C32" s="1" t="s">
@@ -1167,6 +1278,9 @@
       </c>
       <c r="G32" s="4" t="s">
         <v>109</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
@@ -1754,4 +1868,99 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E604627B-13DA-4606-B65D-5E7A80F9DCFF}">
+  <dimension ref="B1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="14">
+        <v>45748</v>
+      </c>
+      <c r="E2" s="14">
+        <v>45777</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>